<commit_message>
changed TTL circuit for LoRa
</commit_message>
<xml_diff>
--- a/Altium project/cSLIM-shield/Project Outputs for cSLIM-shield/BOM/Bill of Materials-cSLIM-shield.xlsx
+++ b/Altium project/cSLIM-shield/Project Outputs for cSLIM-shield/BOM/Bill of Materials-cSLIM-shield.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vetleba\Documents\SKOLE\Fordypningsprosjekt\IoF\Altium project\cSLIM-shield\Project Outputs for cSLIM-shield\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4E3ED57-1B1C-4202-96B0-E92FC86DA331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC52D5C1-A743-49DF-919A-5AB2FD3D0D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12735" xr2:uid="{42015810-0AE7-4008-9B25-C1B502286E88}"/>
+    <workbookView xWindow="-18120" yWindow="-120" windowWidth="18240" windowHeight="28440" xr2:uid="{42015810-0AE7-4008-9B25-C1B502286E88}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-cSLIM-shield" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="271">
   <si>
     <t>Comment</t>
   </si>
@@ -447,18 +447,12 @@
     <t>J513</t>
   </si>
   <si>
-    <t>TSW-103-08-S-D</t>
-  </si>
-  <si>
     <t>J516</t>
   </si>
   <si>
     <t>HDRV6W64P254_2X3_762X495X838P</t>
   </si>
   <si>
-    <t>52746-1071</t>
-  </si>
-  <si>
     <t>J802</t>
   </si>
   <si>
@@ -483,21 +477,12 @@
     <t>L-1608</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>9n1</t>
   </si>
   <si>
     <t>L902</t>
   </si>
   <si>
-    <t>LQW18AS10NG0CD</t>
-  </si>
-  <si>
-    <t>L_1</t>
-  </si>
-  <si>
     <t>22nH</t>
   </si>
   <si>
@@ -543,15 +528,6 @@
     <t>LED504, LED505</t>
   </si>
   <si>
-    <t>NetTie</t>
-  </si>
-  <si>
-    <t>NT1201, NT1202</t>
-  </si>
-  <si>
-    <t>NETTIE_FP</t>
-  </si>
-  <si>
     <t>Switch 4-pi. used 1-3 (2-4 not in use)</t>
   </si>
   <si>
@@ -585,9 +561,6 @@
     <t>RESC1608X55N</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>120R</t>
   </si>
   <si>
@@ -733,13 +706,157 @@
   </si>
   <si>
     <t>RV3032C7TAQA</t>
+  </si>
+  <si>
+    <t>HAVE</t>
+  </si>
+  <si>
+    <t>DigiKEY</t>
+  </si>
+  <si>
+    <t>3.3pF</t>
+  </si>
+  <si>
+    <t>NIS</t>
+  </si>
+  <si>
+    <t>6 (M8N)</t>
+  </si>
+  <si>
+    <t>SF72S006VBDR2500</t>
+  </si>
+  <si>
+    <t>M20-9980346</t>
+  </si>
+  <si>
+    <t>0527461071</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>LQG18HH27NJ00D</t>
+  </si>
+  <si>
+    <t>(0402) 20</t>
+  </si>
+  <si>
+    <t>MOUSER</t>
+  </si>
+  <si>
+    <t>LQW18AN9N1D00D</t>
+  </si>
+  <si>
+    <t>LQG18HN1N5S00D</t>
+  </si>
+  <si>
+    <t>LQW18AN22NJ00D</t>
+  </si>
+  <si>
+    <t>197stock</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>RT0603DRD07120RL</t>
+  </si>
+  <si>
+    <t>RC0603JR-07680RL</t>
+  </si>
+  <si>
+    <t>RC0603JR-0715RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07820RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-130RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07330RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07240KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-131ML</t>
+  </si>
+  <si>
+    <t>RC0603JR-07390RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-071KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-071M2L</t>
+  </si>
+  <si>
+    <t>RC0603FR-073KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-1310RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-0733RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-0749R9L</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-074K7L</t>
+  </si>
+  <si>
+    <t>CL10B104KB8NNNL</t>
+  </si>
+  <si>
+    <t>0603N120J500CT</t>
+  </si>
+  <si>
+    <t>CL10B103KB8NNNC</t>
+  </si>
+  <si>
+    <t>CL10A105KO8NNNC</t>
+  </si>
+  <si>
+    <t>CL10X106MP8NRNC</t>
+  </si>
+  <si>
+    <t>CL10A226KQ8NRNE</t>
+  </si>
+  <si>
+    <t>CL10C1R8BB8NNNC</t>
+  </si>
+  <si>
+    <t>CL10A105KB8NNNC</t>
+  </si>
+  <si>
+    <t>CL10C101JB8NNNC</t>
+  </si>
+  <si>
+    <t>CL10C150JB81PNC</t>
+  </si>
+  <si>
+    <t>GRM188D70E476ME01D</t>
+  </si>
+  <si>
+    <t>CL10A475KQ8NNNC</t>
+  </si>
+  <si>
+    <t>CL10C3R3CB81PNC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,8 +864,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -758,6 +881,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,12 +924,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,16 +1248,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727B3C40-1C4E-4F64-A1B9-E89BE380D209}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1137,8 +1284,17 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1157,8 +1313,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1172,13 +1331,16 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="F3" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="5"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1192,13 +1354,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>259</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="5"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1212,13 +1377,16 @@
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>260</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="5"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -1232,13 +1400,16 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>261</v>
       </c>
       <c r="F6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="5"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1252,13 +1423,16 @@
         <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>262</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="5"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1272,13 +1446,16 @@
         <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>263</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="5"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1292,13 +1469,16 @@
         <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>264</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="5"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1317,8 +1497,13 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="6"/>
+      <c r="H10" s="5">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1332,13 +1517,16 @@
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>265</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="5"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1352,13 +1540,16 @@
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>266</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1372,13 +1563,16 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>267</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="5"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1392,13 +1586,16 @@
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>268</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="5"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1412,13 +1609,16 @@
         <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>269</v>
       </c>
       <c r="F15" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="5"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1432,13 +1632,18 @@
         <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
+        <v>270</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -1457,8 +1662,11 @@
       <c r="F17" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1477,8 +1685,15 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H18" s="5">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
@@ -1497,8 +1712,11 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="5"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
@@ -1517,8 +1735,13 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+      <c r="H20" s="5">
+        <v>4</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1537,8 +1760,13 @@
       <c r="F21" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5">
+        <v>13</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>57</v>
       </c>
@@ -1557,8 +1785,11 @@
       <c r="F22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
@@ -1577,8 +1808,15 @@
       <c r="F23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -1597,8 +1835,15 @@
       <c r="F24" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H24" s="5">
+        <v>12</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>66</v>
       </c>
@@ -1617,8 +1862,15 @@
       <c r="F25" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H25" s="5">
+        <v>12</v>
+      </c>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>70</v>
       </c>
@@ -1637,8 +1889,15 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H26" s="5">
+        <v>4</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>73</v>
       </c>
@@ -1657,8 +1916,15 @@
       <c r="F27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>76</v>
       </c>
@@ -1677,8 +1943,15 @@
       <c r="F28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H28" s="5">
+        <v>4</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>79</v>
       </c>
@@ -1697,8 +1970,13 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5">
+        <v>4</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>82</v>
       </c>
@@ -1717,8 +1995,15 @@
       <c r="F30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>85</v>
       </c>
@@ -1737,8 +2022,11 @@
       <c r="F31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="5"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>89</v>
       </c>
@@ -1757,8 +2045,15 @@
       <c r="F32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H32" s="5">
+        <v>4</v>
+      </c>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>92</v>
       </c>
@@ -1777,8 +2072,11 @@
       <c r="F33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="5"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>96</v>
       </c>
@@ -1797,8 +2095,11 @@
       <c r="F34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="5"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>98</v>
       </c>
@@ -1817,8 +2118,11 @@
       <c r="F35" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="5"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>98</v>
       </c>
@@ -1837,8 +2141,11 @@
       <c r="F36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="5"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>106</v>
       </c>
@@ -1857,8 +2164,11 @@
       <c r="F37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="5"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>110</v>
       </c>
@@ -1877,8 +2187,11 @@
       <c r="F38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="5"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>114</v>
       </c>
@@ -1897,8 +2210,13 @@
       <c r="F39" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="1"/>
+      <c r="H39" s="5">
+        <v>4</v>
+      </c>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
@@ -1917,8 +2235,11 @@
       <c r="F40" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="5"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>121</v>
       </c>
@@ -1937,8 +2258,13 @@
       <c r="F41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="5"/>
+      <c r="H41" s="5">
+        <v>4</v>
+      </c>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>124</v>
       </c>
@@ -1957,8 +2283,13 @@
       <c r="F42" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="5"/>
+      <c r="H42" s="5">
+        <v>10</v>
+      </c>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>127</v>
       </c>
@@ -1977,8 +2308,13 @@
       <c r="F43" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="5"/>
+      <c r="H43" s="5">
+        <v>4</v>
+      </c>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>131</v>
       </c>
@@ -1997,10 +2333,15 @@
       <c r="F44" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="5"/>
+      <c r="H44" s="5">
+        <v>28</v>
+      </c>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>99</v>
@@ -2017,746 +2358,906 @@
       <c r="F45" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="5"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>136</v>
+        <v>229</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>136</v>
+        <v>229</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="5"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>139</v>
+        <v>230</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5">
+        <v>13</v>
+      </c>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H48" s="5">
+        <v>4</v>
+      </c>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="5"/>
+      <c r="H49" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F49" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>152</v>
+        <v>235</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="5"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>148</v>
+        <v>237</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="5"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="5"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="5">
+        <v>4</v>
+      </c>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="B54" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="E54" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="5">
+        <v>4</v>
+      </c>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="B55" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5">
+        <v>4</v>
+      </c>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B56" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="F54" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F55" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="F56" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F57" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="1"/>
+      <c r="H56" s="5">
+        <v>8</v>
+      </c>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F58" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="5"/>
+      <c r="H58" s="5">
+        <v>8</v>
+      </c>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H59" s="5">
+        <v>12</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>182</v>
+        <v>239</v>
       </c>
       <c r="F60" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="5"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>182</v>
+        <v>240</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="5"/>
+      <c r="H61" s="5">
+        <v>8</v>
+      </c>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>182</v>
+        <v>241</v>
       </c>
       <c r="F62" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="5"/>
+      <c r="H62" s="5">
+        <v>100</v>
+      </c>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="F63" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="5"/>
+      <c r="H63" s="1">
+        <v>3</v>
+      </c>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="F64" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="5"/>
+      <c r="H64" s="5">
+        <v>100</v>
+      </c>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>182</v>
+        <v>243</v>
       </c>
       <c r="F65" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="5"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>182</v>
+        <v>245</v>
       </c>
       <c r="F66" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="5"/>
+      <c r="H66" s="5">
+        <v>20</v>
+      </c>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
       <c r="F67" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="5"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>182</v>
+        <v>247</v>
       </c>
       <c r="F68" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="5"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>182</v>
+        <v>248</v>
       </c>
       <c r="F69" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="5"/>
+      <c r="H69" s="5">
+        <v>8</v>
+      </c>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>182</v>
+        <v>249</v>
       </c>
       <c r="F70" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="5"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="F71" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="5"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>182</v>
+        <v>251</v>
       </c>
       <c r="F72" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="5"/>
+      <c r="H72" s="5">
+        <v>8</v>
+      </c>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>182</v>
+        <v>252</v>
       </c>
       <c r="F73" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="5"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>182</v>
+        <v>253</v>
       </c>
       <c r="F74" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="5"/>
+      <c r="H74" s="5">
+        <v>20</v>
+      </c>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>182</v>
+        <v>254</v>
       </c>
       <c r="F75" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="5"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>182</v>
+        <v>255</v>
       </c>
       <c r="F76" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="5"/>
+      <c r="H76" s="5">
+        <v>50</v>
+      </c>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>182</v>
+        <v>256</v>
       </c>
       <c r="F77" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="5"/>
+      <c r="H77" s="5">
+        <v>100</v>
+      </c>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>182</v>
+        <v>257</v>
       </c>
       <c r="F78" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="5"/>
+      <c r="H78" s="5">
+        <v>100</v>
+      </c>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="F79" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="5"/>
+      <c r="H79" s="5">
+        <v>4</v>
+      </c>
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F80" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H80" s="5">
+        <v>4</v>
+      </c>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E81" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1</v>
+      </c>
+      <c r="G81" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="F81" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H81" s="5">
+        <v>5</v>
+      </c>
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F82" s="1">
         <v>1</v>
       </c>
+      <c r="G82" s="1"/>
+      <c r="H82" s="5">
+        <v>4</v>
+      </c>
+      <c r="I82" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>